<commit_message>
refactored RWS, a.o. according to Martijns suggestion.
</commit_message>
<xml_diff>
--- a/NewFrontend/RWS/Kabeladministratie (fout).xlsx
+++ b/NewFrontend/RWS/Kabeladministratie (fout).xlsx
@@ -72,15 +72,9 @@
     <t>CAT 5E</t>
   </si>
   <si>
-    <t>kabelVanInstallatie</t>
-  </si>
-  <si>
     <t>Installatie</t>
   </si>
   <si>
-    <t>kabelNaarInstallatie</t>
-  </si>
-  <si>
     <t>[Installaties]</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>+TE61W01-U73.12</t>
+  </si>
+  <si>
+    <t>vanInst</t>
+  </si>
+  <si>
+    <t>naarInst</t>
   </si>
 </sst>
 </file>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,11 +659,11 @@
         <v>14</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="7" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G1" s="8"/>
     </row>
@@ -678,16 +678,16 @@
         <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -702,14 +702,14 @@
         <v>16</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" ref="E3:E14" si="0">IF($D3="","",VLOOKUP($D3,$A$26:$B$39,2,FALSE))</f>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4" t="str">
         <f t="shared" ref="G3:G14" si="1">IF($F3="","",VLOOKUP($F3,$A$26:$B$39,2,FALSE))</f>
@@ -728,14 +728,14 @@
         <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -754,14 +754,14 @@
         <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" s="4" t="str">
         <f t="shared" si="1"/>
@@ -780,14 +780,14 @@
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -806,14 +806,14 @@
         <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -832,14 +832,14 @@
         <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="4" t="str">
         <f t="shared" si="1"/>
@@ -858,14 +858,14 @@
         <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G9" s="4" t="str">
         <f t="shared" si="1"/>
@@ -884,14 +884,14 @@
         <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G10" s="4" t="str">
         <f t="shared" si="1"/>
@@ -910,14 +910,14 @@
         <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="4" t="str">
         <f t="shared" si="1"/>
@@ -936,14 +936,14 @@
         <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G12" s="4" t="str">
         <f t="shared" si="1"/>
@@ -956,7 +956,7 @@
         <v>Kabel_13-69-061</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="str">
@@ -981,14 +981,14 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G14" s="4" t="str">
         <f t="shared" si="1"/>
@@ -1120,7 +1120,7 @@
         <v/>
       </c>
       <c r="F21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G21" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1140,7 +1140,7 @@
         <v>16</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1156,130 +1156,130 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update van handleiding en bestanden.
</commit_message>
<xml_diff>
--- a/NewFrontend/RWS/Kabeladministratie (fout).xlsx
+++ b/NewFrontend/RWS/Kabeladministratie (fout).xlsx
@@ -11,15 +11,12 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>13-69-051</t>
   </si>
@@ -157,6 +154,30 @@
   </si>
   <si>
     <t>naarInst</t>
+  </si>
+  <si>
+    <t>13-69-063</t>
+  </si>
+  <si>
+    <t>13-69-064</t>
+  </si>
+  <si>
+    <t>13-69-065</t>
+  </si>
+  <si>
+    <t>13-69-066</t>
+  </si>
+  <si>
+    <t>13-69-067</t>
+  </si>
+  <si>
+    <t>13-69-068</t>
+  </si>
+  <si>
+    <t>13-69-069</t>
+  </si>
+  <si>
+    <t>13-69-070</t>
   </si>
 </sst>
 </file>
@@ -285,62 +306,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Blad1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>13-69-063</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>13-69-064</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>13-69-065</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>13-69-066</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>13-69-067</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>13-69-068</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>13-69-069</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>13-69-070</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1000,9 +965,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-063</v>
       </c>
-      <c r="B15" s="5" t="str">
-        <f>[1]Blad1!$A14</f>
-        <v>13-69-063</v>
+      <c r="B15" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" ref="E15:E22" si="3">IF($D15="","",VLOOKUP($D15,$A$26:$B$39,2,FALSE))</f>
@@ -1018,9 +982,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-064</v>
       </c>
-      <c r="B16" s="5" t="str">
-        <f>[1]Blad1!$A15</f>
-        <v>13-69-064</v>
+      <c r="B16" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1036,9 +999,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-065</v>
       </c>
-      <c r="B17" s="5" t="str">
-        <f>[1]Blad1!$A16</f>
-        <v>13-69-065</v>
+      <c r="B17" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1054,9 +1016,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-066</v>
       </c>
-      <c r="B18" s="5" t="str">
-        <f>[1]Blad1!$A17</f>
-        <v>13-69-066</v>
+      <c r="B18" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1072,9 +1033,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-067</v>
       </c>
-      <c r="B19" s="5" t="str">
-        <f>[1]Blad1!$A18</f>
-        <v>13-69-067</v>
+      <c r="B19" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1090,9 +1050,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-068</v>
       </c>
-      <c r="B20" s="5" t="str">
-        <f>[1]Blad1!$A19</f>
-        <v>13-69-068</v>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1108,9 +1067,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-069</v>
       </c>
-      <c r="B21" s="5" t="str">
-        <f>[1]Blad1!$A20</f>
-        <v>13-69-069</v>
+      <c r="B21" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>16</v>
@@ -1132,9 +1090,8 @@
         <f t="shared" si="2"/>
         <v>Kabel_13-69-070</v>
       </c>
-      <c r="B22" s="5" t="str">
-        <f>[1]Blad1!$A21</f>
-        <v>13-69-070</v>
+      <c r="B22" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>16</v>

</xml_diff>